<commit_message>
middleware updated to handle new token-structure changes
</commit_message>
<xml_diff>
--- a/Project-Service-implementation-Script/Sample Templates/ProgramTemplate.xlsx
+++ b/Project-Service-implementation-Script/Sample Templates/ProgramTemplate.xlsx
@@ -5,13 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Instructions" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Program Details" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Resource Details" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Program Manager Details" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Instructions" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Program Details" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="Resource Details" sheetId="3" state="visible" r:id="rId5"/>
+    <sheet name="Program Manager Details" sheetId="4" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="88">
   <si>
     <t xml:space="preserve">Template Version : 5.1.0</t>
   </si>
@@ -221,6 +221,12 @@
     <t xml:space="preserve">projectService username/user id/email id/phone no. of Program Designer</t>
   </si>
   <si>
+    <t xml:space="preserve">Tenant ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Org ID</t>
+  </si>
+  <si>
     <t xml:space="preserve">Targeted entities at program level</t>
   </si>
   <si>
@@ -228,6 +234,9 @@
   </si>
   <si>
     <t xml:space="preserve">tncontentcreator@yopmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24</t>
   </si>
   <si>
     <t xml:space="preserve">Indiranagar</t>
@@ -292,9 +301,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="mm\-dd\-yyyy"/>
+    <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="166" formatCode="mm\-dd\-yyyy"/>
   </numFmts>
   <fonts count="13">
     <font>
@@ -519,176 +529,180 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -764,8 +778,114 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -777,646 +897,646 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="38.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="12.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="60.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="6" style="0" width="12.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="35.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="38.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="1" width="12.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="60.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="6" style="1" width="12.88"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="8"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
+      <c r="A7" s="9"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="11"/>
-      <c r="D8" s="12" t="s">
+      <c r="C8" s="12"/>
+      <c r="D8" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="12"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="14"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="15" t="s">
+      <c r="B9" s="15"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="16" t="s">
+      <c r="E9" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="19" t="s">
+      <c r="B10" s="19"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="20" t="s">
+      <c r="E10" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="17" t="s">
+      <c r="A11" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="21"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="19" t="s">
+      <c r="B11" s="22"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="20" t="s">
+      <c r="E11" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="22"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="19" t="s">
+      <c r="B12" s="23"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="20" t="s">
+      <c r="E12" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="17"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11" t="s">
+      <c r="A13" s="18"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="20" t="s">
+      <c r="E13" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="23" t="s">
+      <c r="A14" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="23"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11" t="s">
+      <c r="B14" s="24"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="E14" s="20" t="s">
+      <c r="E14" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="24" t="s">
+      <c r="A15" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="11"/>
-      <c r="D15" s="19" t="s">
+      <c r="C15" s="12"/>
+      <c r="D15" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="E15" s="20" t="s">
+      <c r="E15" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="13" t="s">
+      <c r="A16" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="19" t="s">
+      <c r="B16" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="11"/>
-      <c r="D16" s="19" t="s">
+      <c r="C16" s="12"/>
+      <c r="D16" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="E16" s="20" t="s">
+      <c r="E16" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="25"/>
-      <c r="K16" s="25"/>
-      <c r="L16" s="25"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="26"/>
+      <c r="K16" s="26"/>
+      <c r="L16" s="26"/>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="13" t="s">
+      <c r="A17" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="20" t="s">
+      <c r="B17" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="11"/>
-      <c r="D17" s="19" t="s">
+      <c r="C17" s="12"/>
+      <c r="D17" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="E17" s="20" t="s">
+      <c r="E17" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="2"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="13" t="s">
+      <c r="A18" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="20" t="s">
+      <c r="B18" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="11"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="17" t="s">
+      <c r="A19" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="11"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="13" t="s">
+      <c r="A20" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="B20" s="20" t="s">
+      <c r="B20" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="C20" s="11"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="13" t="s">
+      <c r="A21" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="B21" s="20" t="s">
+      <c r="B21" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="C21" s="11"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4"/>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="13" t="s">
+      <c r="A22" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B22" s="20" t="s">
+      <c r="B22" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="C22" s="11"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
-      <c r="K22" s="3"/>
-      <c r="L22" s="3"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4"/>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="13" t="s">
+      <c r="A23" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="B23" s="20" t="s">
+      <c r="B23" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="C23" s="11"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
-      <c r="K23" s="3"/>
-      <c r="L23" s="3"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="4"/>
+      <c r="K23" s="4"/>
+      <c r="L23" s="4"/>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="17" t="s">
+      <c r="A24" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="B24" s="20" t="s">
+      <c r="B24" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="C24" s="11"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="25"/>
-      <c r="G24" s="25"/>
-      <c r="H24" s="25"/>
-      <c r="I24" s="25"/>
-      <c r="J24" s="25"/>
-      <c r="K24" s="25"/>
-      <c r="L24" s="25"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="26"/>
+      <c r="H24" s="26"/>
+      <c r="I24" s="26"/>
+      <c r="J24" s="26"/>
+      <c r="K24" s="26"/>
+      <c r="L24" s="26"/>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="17" t="s">
+      <c r="A25" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="B25" s="20" t="s">
+      <c r="B25" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="C25" s="11"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
-      <c r="K25" s="3"/>
-      <c r="L25" s="3"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="4"/>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="17" t="s">
+      <c r="A26" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="B26" s="20" t="s">
+      <c r="B26" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="C26" s="11"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
-      <c r="J26" s="3"/>
-      <c r="K26" s="3"/>
-      <c r="L26" s="3"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4"/>
+      <c r="L26" s="4"/>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="17"/>
-      <c r="B27" s="11"/>
-      <c r="C27" s="11"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
-      <c r="I27" s="3"/>
-      <c r="J27" s="3"/>
-      <c r="K27" s="3"/>
-      <c r="L27" s="3"/>
+      <c r="A27" s="18"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="4"/>
+      <c r="K27" s="4"/>
+      <c r="L27" s="4"/>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="26" t="s">
+      <c r="A28" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="B28" s="26"/>
-      <c r="C28" s="11"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
-      <c r="I28" s="3"/>
-      <c r="J28" s="3"/>
-      <c r="K28" s="3"/>
-      <c r="L28" s="3"/>
+      <c r="B28" s="27"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
+      <c r="K28" s="4"/>
+      <c r="L28" s="4"/>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="24" t="s">
+      <c r="A29" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="B29" s="15" t="s">
+      <c r="B29" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C29" s="11"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-      <c r="I29" s="3"/>
-      <c r="J29" s="3"/>
-      <c r="K29" s="3"/>
-      <c r="L29" s="3"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="4"/>
+      <c r="K29" s="4"/>
+      <c r="L29" s="4"/>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="17" t="s">
+      <c r="A30" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="B30" s="20" t="s">
+      <c r="B30" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="C30" s="11"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="3"/>
-      <c r="J30" s="3"/>
-      <c r="K30" s="3"/>
-      <c r="L30" s="3"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4"/>
+      <c r="J30" s="4"/>
+      <c r="K30" s="4"/>
+      <c r="L30" s="4"/>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="17" t="s">
+      <c r="A31" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="B31" s="20" t="s">
+      <c r="B31" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="C31" s="11"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
-      <c r="I31" s="3"/>
-      <c r="J31" s="3"/>
-      <c r="K31" s="3"/>
-      <c r="L31" s="3"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="4"/>
+      <c r="J31" s="4"/>
+      <c r="K31" s="4"/>
+      <c r="L31" s="4"/>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="17" t="s">
+      <c r="A32" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="B32" s="20" t="s">
+      <c r="B32" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="C32" s="11"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
-      <c r="G32" s="3"/>
-      <c r="H32" s="3"/>
-      <c r="I32" s="3"/>
-      <c r="J32" s="3"/>
-      <c r="K32" s="3"/>
-      <c r="L32" s="3"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
+      <c r="I32" s="4"/>
+      <c r="J32" s="4"/>
+      <c r="K32" s="4"/>
+      <c r="L32" s="4"/>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="3"/>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
-      <c r="H33" s="3"/>
-      <c r="I33" s="3"/>
-      <c r="J33" s="3"/>
-      <c r="K33" s="3"/>
-      <c r="L33" s="3"/>
+      <c r="A33" s="4"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="4"/>
+      <c r="I33" s="4"/>
+      <c r="J33" s="4"/>
+      <c r="K33" s="4"/>
+      <c r="L33" s="4"/>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="27"/>
-      <c r="B34" s="27"/>
-      <c r="C34" s="27"/>
-      <c r="D34" s="27"/>
-      <c r="E34" s="27"/>
-      <c r="F34" s="27"/>
-      <c r="G34" s="27"/>
-      <c r="H34" s="3"/>
-      <c r="I34" s="3"/>
-      <c r="J34" s="3"/>
-      <c r="K34" s="3"/>
-      <c r="L34" s="3"/>
+      <c r="A34" s="28"/>
+      <c r="B34" s="28"/>
+      <c r="C34" s="28"/>
+      <c r="D34" s="28"/>
+      <c r="E34" s="28"/>
+      <c r="F34" s="28"/>
+      <c r="G34" s="28"/>
+      <c r="H34" s="4"/>
+      <c r="I34" s="4"/>
+      <c r="J34" s="4"/>
+      <c r="K34" s="4"/>
+      <c r="L34" s="4"/>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="3"/>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
-      <c r="G35" s="3"/>
-      <c r="H35" s="3"/>
-      <c r="I35" s="3"/>
-      <c r="J35" s="3"/>
-      <c r="K35" s="3"/>
-      <c r="L35" s="3"/>
+      <c r="A35" s="4"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="4"/>
+      <c r="I35" s="4"/>
+      <c r="J35" s="4"/>
+      <c r="K35" s="4"/>
+      <c r="L35" s="4"/>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="3"/>
-      <c r="B36" s="3"/>
-      <c r="C36" s="27"/>
-      <c r="D36" s="27"/>
-      <c r="E36" s="27"/>
-      <c r="F36" s="27"/>
-      <c r="G36" s="27"/>
-      <c r="H36" s="27"/>
-      <c r="I36" s="27"/>
-      <c r="J36" s="27"/>
-      <c r="K36" s="27"/>
-      <c r="L36" s="27"/>
+      <c r="A36" s="4"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="28"/>
+      <c r="D36" s="28"/>
+      <c r="E36" s="28"/>
+      <c r="F36" s="28"/>
+      <c r="G36" s="28"/>
+      <c r="H36" s="28"/>
+      <c r="I36" s="28"/>
+      <c r="J36" s="28"/>
+      <c r="K36" s="28"/>
+      <c r="L36" s="28"/>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2407,136 +2527,150 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L1000"/>
+  <dimension ref="A1:N1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="12.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="16.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="15.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="17.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="12" style="0" width="12.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="21.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="1" width="16.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="19.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="17.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="1" width="12.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="15.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="16.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="15.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="17.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="14" style="1" width="12.88"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="28" t="s">
+    <row r="1" customFormat="false" ht="103.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="F1" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="G1" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="H1" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="G1" s="29" t="s">
+      <c r="I1" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="H1" s="29" t="s">
+      <c r="J1" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="I1" s="29" t="s">
+      <c r="K1" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="J1" s="29" t="s">
+      <c r="L1" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="K1" s="29" t="s">
+      <c r="M1" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="L1" s="3"/>
+      <c r="N1" s="4"/>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="30" t="s">
+    <row r="2" customFormat="false" ht="108.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="C2" s="31" t="s">
+      <c r="C2" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="D2" s="30" t="s">
+      <c r="D2" s="32" t="s">
+        <v>64</v>
+      </c>
+      <c r="E2" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="F2" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="E2" s="31" t="s">
+      <c r="G2" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="F2" s="31" t="s">
+      <c r="H2" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="30" t="s">
+      <c r="I2" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="31" t="s">
+      <c r="J2" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="I2" s="32" t="s">
+      <c r="K2" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="J2" s="31" t="s">
+      <c r="L2" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="K2" s="31" t="s">
+      <c r="M2" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="L2" s="3"/>
+      <c r="N2" s="4"/>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B3" s="33" t="s">
-        <v>65</v>
-      </c>
-      <c r="C3" s="34" t="s">
+    <row r="3" customFormat="false" ht="61.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
         <v>66</v>
       </c>
+      <c r="B3" s="34" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" s="34" t="n">
+        <v>24</v>
+      </c>
       <c r="D3" s="35" t="s">
-        <v>66</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="F3" s="34" t="s">
         <v>68</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="E3" s="36" t="s">
         <v>69</v>
       </c>
+      <c r="F3" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>70</v>
+      </c>
       <c r="H3" s="36" t="s">
-        <v>70</v>
-      </c>
-      <c r="I3" s="34" t="s">
         <v>71</v>
       </c>
+      <c r="I3" s="4" t="s">
+        <v>72</v>
+      </c>
       <c r="J3" s="37" t="s">
-        <v>72</v>
-      </c>
-      <c r="K3" s="34" t="s">
         <v>73</v>
+      </c>
+      <c r="K3" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="L3" s="38" t="s">
+        <v>75</v>
+      </c>
+      <c r="M3" s="36" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -3538,11 +3672,11 @@
     <row r="1000" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="C3" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="E3" type="list">
       <formula1>"Andaman &amp; Nicobar Islands,Andhra Pradesh,Arunachal Pradesh,Assam,Bihar,Chandigarh,Chhattisgarh,Dadra and Nagar Haveli and Daman and Diu,Delhi,Goa,Gujarat,Haryana,Himachal Pradesh,Jammu And Kashmir,Jharkhand,Karnataka,Kerala,Ladakh,Lakshadweep,Madhya Prade"&amp;"sh,Maharashtra,Manipur,Meghalaya,Mizoram,Nagaland,Odisha,Puducherry,Punjab,Rajasthan,Sikkim,Tamil Nadu,Telangana,Tripura,Uttar Pradesh,Uttarakhand,West Bengal"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="H3" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="J3" type="list">
       <formula1>#ref!</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -3558,107 +3692,107 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:I1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="19.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="9" style="0" width="12.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="23.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="22.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="23.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="19.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="20.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="20.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="15.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="19.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="9" style="1" width="12.88"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="D1" s="29" t="s">
+      <c r="C1" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="E1" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="29" t="s">
-        <v>75</v>
-      </c>
-      <c r="G1" s="29" t="s">
+      <c r="F1" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="H1" s="29" t="s">
+      <c r="H1" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="I1" s="3"/>
+      <c r="I1" s="4"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="38" t="s">
+      <c r="C2" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="38" t="s">
+      <c r="D2" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="31" t="s">
+      <c r="E2" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="32" t="s">
+      <c r="F2" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="G2" s="32" t="s">
+      <c r="G2" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="H2" s="32" t="s">
+      <c r="H2" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="I2" s="3"/>
+      <c r="I2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="40" t="s">
+        <v>79</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" s="41" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E3" s="37" t="s">
+        <v>73</v>
+      </c>
+      <c r="F3" s="36" t="s">
+        <v>83</v>
+      </c>
+      <c r="G3" s="38" t="s">
+        <v>75</v>
+      </c>
+      <c r="H3" s="36" t="s">
         <v>76</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C3" s="40" t="s">
-        <v>78</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="E3" s="36" t="s">
-        <v>70</v>
-      </c>
-      <c r="F3" s="34" t="s">
-        <v>80</v>
-      </c>
-      <c r="G3" s="37" t="s">
-        <v>72</v>
-      </c>
-      <c r="H3" s="34" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -4684,7 +4818,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -4696,62 +4830,62 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="1" style="0" width="12.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="1" style="1" width="12.88"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="D1" s="3"/>
+      <c r="D1" s="4"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="38" t="s">
-        <v>81</v>
-      </c>
-      <c r="B2" s="41" t="s">
+      <c r="A2" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="41" t="s">
+      <c r="C2" s="42" t="s">
         <v>58</v>
       </c>
-      <c r="D2" s="3"/>
+      <c r="D2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="B3" s="42" t="s">
-        <v>83</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
+      <c r="A3" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" s="43" t="s">
+        <v>86</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="B4" s="33" t="s">
-        <v>84</v>
-      </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
+      <c r="A4" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B4" s="34" t="s">
+        <v>87</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="B5" s="33" t="s">
-        <v>65</v>
-      </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
+      <c r="A5" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B5" s="34" t="s">
+        <v>67</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>